<commit_message>
Moved all GUI code to separate class, starting coding asynchronous coding
</commit_message>
<xml_diff>
--- a/res_next_email_list.xlsx
+++ b/res_next_email_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="96" windowWidth="18180" windowHeight="8496"/>
+    <workbookView xWindow="390" yWindow="90" windowWidth="18180" windowHeight="8490"/>
   </bookViews>
   <sheets>
     <sheet name="Лист2" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="206">
   <si>
     <t>email</t>
   </si>
@@ -626,25 +626,16 @@
     <t>Фёдор</t>
   </si>
   <si>
-    <t>1534</t>
-  </si>
-  <si>
     <t>i0808</t>
   </si>
   <si>
     <t>Полина</t>
   </si>
   <si>
-    <t>368</t>
-  </si>
-  <si>
     <t>i1012</t>
   </si>
   <si>
     <t>Владислав</t>
-  </si>
-  <si>
-    <t>1900</t>
   </si>
   <si>
     <t>субботу 29 апреля</t>
@@ -798,7 +789,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -819,16 +810,10 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -844,12 +829,48 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="27">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -930,35 +951,6 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -979,21 +971,21 @@
     <tableColumn id="2" name="Фамилия"/>
     <tableColumn id="3" name="Имя"/>
     <tableColumn id="4" name="Ауд"/>
-    <tableColumn id="5" name="Школа"/>
-    <tableColumn id="6" name="Год р."/>
-    <tableColumn id="7" name="email" dataDxfId="24"/>
+    <tableColumn id="5" name="Школа" dataDxfId="2"/>
+    <tableColumn id="6" name="Год р." dataDxfId="0"/>
+    <tableColumn id="7" name="email" dataDxfId="1"/>
     <tableColumn id="8" name="а"/>
-    <tableColumn id="9" name="subject" dataDxfId="23">
+    <tableColumn id="9" name="subject" dataDxfId="26">
       <calculatedColumnFormula>"Собеседования в 7-й математический класс 179-й школы"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" name="|" dataDxfId="22">
+    <tableColumn id="40" name="|" dataDxfId="25">
       <calculatedColumnFormula>"|"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="attach1" dataDxfId="21">
-      <calculatedColumnFormula>"C:\Dropbox\M2021-sob\Собеседование в 7-й класс, 2017\_Задачи собеседований\sob10.pdf"</calculatedColumnFormula>
+    <tableColumn id="10" name="attach1" dataDxfId="24">
+      <calculatedColumnFormula>"C:\Dropbox\M2021-sob\Собеседование в 7-й класс, 2017\_Задачи собеседований\sob9.pdf"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="attach2" dataDxfId="20"/>
-    <tableColumn id="41" name="/" dataDxfId="19">
+    <tableColumn id="11" name="attach2" dataDxfId="23"/>
+    <tableColumn id="41" name="/" dataDxfId="22">
       <calculatedColumnFormula>"."</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" name="next_date"/>
@@ -1005,18 +997,18 @@
     <tableColumn id="18" name="p6"/>
     <tableColumn id="19" name="p7"/>
     <tableColumn id="20" name="p8"/>
-    <tableColumn id="21" name="ptot" dataDxfId="18">
+    <tableColumn id="21" name="ptot" dataDxfId="21">
       <calculatedColumnFormula>ROUND(SUM(O2:V2),2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="c11" dataDxfId="17"/>
-    <tableColumn id="23" name="c12" dataDxfId="16"/>
-    <tableColumn id="24" name="c13" dataDxfId="15"/>
-    <tableColumn id="25" name="c14" dataDxfId="14"/>
-    <tableColumn id="26" name="c15" dataDxfId="13"/>
-    <tableColumn id="27" name="c16" dataDxfId="12"/>
-    <tableColumn id="28" name="c17" dataDxfId="11"/>
-    <tableColumn id="29" name="c18" dataDxfId="10"/>
-    <tableColumn id="30" name="c1tot" dataDxfId="9">
+    <tableColumn id="22" name="c11" dataDxfId="20"/>
+    <tableColumn id="23" name="c12" dataDxfId="19"/>
+    <tableColumn id="24" name="c13" dataDxfId="18"/>
+    <tableColumn id="25" name="c14" dataDxfId="17"/>
+    <tableColumn id="26" name="c15" dataDxfId="16"/>
+    <tableColumn id="27" name="c16" dataDxfId="15"/>
+    <tableColumn id="28" name="c17" dataDxfId="14"/>
+    <tableColumn id="29" name="c18" dataDxfId="13"/>
+    <tableColumn id="30" name="c1tot" dataDxfId="12">
       <calculatedColumnFormula>IF(X2="+",1,IF(X2="+.",1,IF(X2="+-",0.8,IF(X2="+/2",0.5,IF(X2="-+",0.1,IF(X2="-.",0,IF(X2="-",0,IF(X2="0",0,IF(X2="",0,"?")))))))))+
 IF(Y2="+",1,IF(Y2="+.",1,IF(Y2="+-",0.8,IF(Y2="+/2",0.5,IF(Y2="-+",0.1,IF(Y2="-.",0,IF(Y2="-",0,IF(Y2="0",0,IF(Y2="",0,"?")))))))))+
 IF(Z2="+",1,IF(Z2="+.",1,IF(Z2="+-",0.8,IF(Z2="+/2",0.5,IF(Z2="-+",0.1,IF(Z2="-.",0,IF(Z2="-",0,IF(Z2="0",0,IF(Z2="",0,"?")))))))))+
@@ -1026,31 +1018,31 @@
 IF(AD2="+",1,IF(AD2="+.",1,IF(AD2="+-",0.8,IF(AD2="+/2",0.5,IF(AD2="-+",0.1,IF(AD2="-.",0,IF(AD2="-",0,IF(AD2="0",0,IF(AD2="",0,"?")))))))))+
 IF(AE2="+",1,IF(AE2="+.",1,IF(AE2="+-",0.8,IF(AE2="+/2",0.5,IF(AE2="-+",0.1,IF(AE2="-.",0,IF(AE2="-",0,IF(AE2="0",0,IF(AE2="",0,"?")))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" name="c31" dataDxfId="8">
+    <tableColumn id="31" name="c31" dataDxfId="11">
       <calculatedColumnFormula>ROUND(IF(X2="+",1,IF(X2="+.",1,IF(X2="+-",0.8,IF(X2="+/2",0.5,IF(X2="-+",0.1,IF(X2="-.",0,IF(X2="-",0,IF(X2="0",0,IF(X2="",0,"?")))))))))*#REF!,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" name="c32" dataDxfId="7">
+    <tableColumn id="32" name="c32" dataDxfId="10">
       <calculatedColumnFormula>ROUND(IF(Y2="+",1,IF(Y2="+.",1,IF(Y2="+-",0.8,IF(Y2="+/2",0.5,IF(Y2="-+",0.1,IF(Y2="-.",0,IF(Y2="-",0,IF(Y2="0",0,IF(Y2="",0,"?")))))))))*#REF!,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" name="c33" dataDxfId="6">
+    <tableColumn id="33" name="c33" dataDxfId="9">
       <calculatedColumnFormula>ROUND(IF(Z2="+",1,IF(Z2="+.",1,IF(Z2="+-",0.8,IF(Z2="+/2",0.5,IF(Z2="-+",0.1,IF(Z2="-.",0,IF(Z2="-",0,IF(Z2="0",0,IF(Z2="",0,"?")))))))))*#REF!,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" name="c34" dataDxfId="5">
+    <tableColumn id="34" name="c34" dataDxfId="8">
       <calculatedColumnFormula>ROUND(IF(AA2="+",1,IF(AA2="+.",1,IF(AA2="+-",0.8,IF(AA2="+/2",0.5,IF(AA2="-+",0.1,IF(AA2="-.",0,IF(AA2="-",0,IF(AA2="0",0,IF(AA2="",0,"?")))))))))*#REF!,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="c35" dataDxfId="4">
+    <tableColumn id="35" name="c35" dataDxfId="7">
       <calculatedColumnFormula>ROUND(IF(AB2="+",1,IF(AB2="+.",1,IF(AB2="+-",0.8,IF(AB2="+/2",0.5,IF(AB2="-+",0.1,IF(AB2="-.",0,IF(AB2="-",0,IF(AB2="0",0,IF(AB2="",0,"?")))))))))*#REF!,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" name="c36" dataDxfId="3">
+    <tableColumn id="36" name="c36" dataDxfId="6">
       <calculatedColumnFormula>ROUND(IF(AC2="+",1,IF(AC2="+.",1,IF(AC2="+-",0.8,IF(AC2="+/2",0.5,IF(AC2="-+",0.1,IF(AC2="-.",0,IF(AC2="-",0,IF(AC2="0",0,IF(AC2="",0,"?")))))))))*#REF!,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" name="c37" dataDxfId="2">
+    <tableColumn id="37" name="c37" dataDxfId="5">
       <calculatedColumnFormula>ROUND(IF(AD2="+",1,IF(AD2="+.",1,IF(AD2="+-",0.8,IF(AD2="+/2",0.5,IF(AD2="-+",0.1,IF(AD2="-.",0,IF(AD2="-",0,IF(AD2="0",0,IF(AD2="",0,"?")))))))))*#REF!,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" name="c38" dataDxfId="1">
+    <tableColumn id="38" name="c38" dataDxfId="4">
       <calculatedColumnFormula>ROUND(IF(AE2="+",1,IF(AE2="+.",1,IF(AE2="+-",0.8,IF(AE2="+/2",0.5,IF(AE2="-+",0.1,IF(AE2="-.",0,IF(AE2="-",0,IF(AE2="0",0,IF(AE2="",0,"?")))))))))*#REF!,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" name="c3tot" dataDxfId="0">
+    <tableColumn id="39" name="c3tot" dataDxfId="3">
       <calculatedColumnFormula>ROUND(SUM(AG2:AN2),2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1351,32 +1343,32 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.88671875" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="82.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" customWidth="1"/>
-    <col min="13" max="13" width="1.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.109375" customWidth="1"/>
-    <col min="15" max="19" width="4.88671875" customWidth="1"/>
+    <col min="11" max="11" width="82.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="19" width="4.85546875" customWidth="1"/>
     <col min="20" max="22" width="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.33203125" customWidth="1"/>
-    <col min="24" max="28" width="5.6640625" style="18" customWidth="1"/>
-    <col min="29" max="31" width="9.109375" style="18"/>
-    <col min="33" max="40" width="8.88671875" style="15"/>
-    <col min="41" max="41" width="8.88671875" style="16"/>
+    <col min="23" max="23" width="6.28515625" customWidth="1"/>
+    <col min="24" max="28" width="5.7109375" style="16" customWidth="1"/>
+    <col min="29" max="31" width="9.140625" style="16"/>
+    <col min="33" max="40" width="8.85546875" style="13"/>
+    <col min="41" max="41" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>31</v>
       </c>
@@ -1446,82 +1438,82 @@
       <c r="W1" t="s">
         <v>86</v>
       </c>
-      <c r="X1" s="18" t="s">
+      <c r="X1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="Y1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="Z1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AA1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AB1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AC1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="AD1" s="18" t="s">
+      <c r="AD1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="18" t="s">
+      <c r="AE1" s="16" t="s">
         <v>10</v>
       </c>
       <c r="AF1" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AG1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AH1" s="15" t="s">
+      <c r="AH1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="AI1" s="15" t="s">
+      <c r="AI1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="AJ1" s="15" t="s">
+      <c r="AJ1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AK1" s="15" t="s">
+      <c r="AK1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="AL1" s="15" t="s">
+      <c r="AL1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AM1" s="15" t="s">
+      <c r="AM1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="AN1" s="15" t="s">
+      <c r="AN1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="AO1" s="16" t="s">
+      <c r="AO1" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="D2" s="11">
+        <v>194</v>
+      </c>
+      <c r="D2" s="10">
         <v>307</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="F2" s="10">
+      <c r="E2" s="9">
+        <v>1900</v>
+      </c>
+      <c r="F2" s="9">
         <v>2004</v>
       </c>
-      <c r="G2" s="20" t="s">
-        <v>201</v>
+      <c r="G2" s="18" t="s">
+        <v>198</v>
       </c>
       <c r="I2" s="1" t="str">
         <f t="shared" ref="I2" si="0">"Собеседования в 7-й математический класс 179-й школы"</f>
@@ -1532,15 +1524,15 @@
         <v>|</v>
       </c>
       <c r="K2" t="str">
-        <f t="shared" ref="K2:K5" si="2">"C:\Dropbox\M2021-sob\Собеседование в 7-й класс, 2017\_Задачи собеседований\sob10.pdf"</f>
-        <v>C:\Dropbox\M2021-sob\Собеседование в 7-й класс, 2017\_Задачи собеседований\sob10.pdf</v>
+        <f t="shared" ref="K2:K5" si="2">"C:\Dropbox\M2021-sob\Собеседование в 7-й класс, 2017\_Задачи собеседований\sob9.pdf"</f>
+        <v>C:\Dropbox\M2021-sob\Собеседование в 7-й класс, 2017\_Задачи собеседований\sob9.pdf</v>
       </c>
       <c r="M2" t="str">
         <f t="shared" ref="M2:M3" si="3">"."</f>
         <v>.</v>
       </c>
       <c r="N2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="O2">
         <v>0.82</v>
@@ -1567,25 +1559,25 @@
         <f t="shared" ref="W2:W5" si="4">ROUND(SUM(O2:V2),2)</f>
         <v>10.130000000000001</v>
       </c>
-      <c r="X2" s="18" t="s">
+      <c r="X2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="18" t="s">
+      <c r="Y2" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="Z2" s="18" t="s">
+      <c r="Z2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AA2" s="18" t="s">
+      <c r="AA2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AB2" s="18" t="s">
+      <c r="AB2" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="AC2" s="18" t="s">
+      <c r="AC2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AD2" s="18" t="s">
+      <c r="AD2" s="16" t="s">
         <v>20</v>
       </c>
       <c r="AF2" s="3">
@@ -1599,64 +1591,64 @@
 IF(AE2="+",1,IF(AE2="+.",1,IF(AE2="+-",0.8,IF(AE2="+/2",0.5,IF(AE2="-+",0.1,IF(AE2="-.",0,IF(AE2="-",0,IF(AE2="0",0,IF(AE2="",0,"?")))))))))</f>
         <v>5</v>
       </c>
-      <c r="AG2" s="15" t="e">
+      <c r="AG2" s="13" t="e">
         <f>ROUND(IF(X2="+",1,IF(X2="+.",1,IF(X2="+-",0.8,IF(X2="+/2",0.5,IF(X2="-+",0.1,IF(X2="-.",0,IF(X2="-",0,IF(X2="0",0,IF(X2="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AH2" s="15" t="e">
+      <c r="AH2" s="13" t="e">
         <f>ROUND(IF(Y2="+",1,IF(Y2="+.",1,IF(Y2="+-",0.8,IF(Y2="+/2",0.5,IF(Y2="-+",0.1,IF(Y2="-.",0,IF(Y2="-",0,IF(Y2="0",0,IF(Y2="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AI2" s="15" t="e">
+      <c r="AI2" s="13" t="e">
         <f>ROUND(IF(Z2="+",1,IF(Z2="+.",1,IF(Z2="+-",0.8,IF(Z2="+/2",0.5,IF(Z2="-+",0.1,IF(Z2="-.",0,IF(Z2="-",0,IF(Z2="0",0,IF(Z2="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AJ2" s="15" t="e">
+      <c r="AJ2" s="13" t="e">
         <f>ROUND(IF(AA2="+",1,IF(AA2="+.",1,IF(AA2="+-",0.8,IF(AA2="+/2",0.5,IF(AA2="-+",0.1,IF(AA2="-.",0,IF(AA2="-",0,IF(AA2="0",0,IF(AA2="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AK2" s="15" t="e">
+      <c r="AK2" s="13" t="e">
         <f>ROUND(IF(AB2="+",1,IF(AB2="+.",1,IF(AB2="+-",0.8,IF(AB2="+/2",0.5,IF(AB2="-+",0.1,IF(AB2="-.",0,IF(AB2="-",0,IF(AB2="0",0,IF(AB2="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL2" s="15" t="e">
+      <c r="AL2" s="13" t="e">
         <f>ROUND(IF(AC2="+",1,IF(AC2="+.",1,IF(AC2="+-",0.8,IF(AC2="+/2",0.5,IF(AC2="-+",0.1,IF(AC2="-.",0,IF(AC2="-",0,IF(AC2="0",0,IF(AC2="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AM2" s="15" t="e">
+      <c r="AM2" s="13" t="e">
         <f>ROUND(IF(AD2="+",1,IF(AD2="+.",1,IF(AD2="+-",0.8,IF(AD2="+/2",0.5,IF(AD2="-+",0.1,IF(AD2="-.",0,IF(AD2="-",0,IF(AD2="0",0,IF(AD2="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AN2" s="15" t="e">
+      <c r="AN2" s="13" t="e">
         <f>ROUND(IF(AE2="+",1,IF(AE2="+.",1,IF(AE2="+-",0.8,IF(AE2="+/2",0.5,IF(AE2="-+",0.1,IF(AE2="-.",0,IF(AE2="-",0,IF(AE2="0",0,IF(AE2="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AO2" s="16" t="e">
+      <c r="AO2" s="14" t="e">
         <f t="shared" ref="AO2:AO3" si="6">ROUND(SUM(AG2:AN2),2)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>189</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>305</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="F3" s="13">
+      <c r="E3" s="9">
+        <v>1534</v>
+      </c>
+      <c r="F3" s="19">
         <v>2004</v>
       </c>
-      <c r="G3" s="20" t="s">
-        <v>202</v>
+      <c r="G3" s="18" t="s">
+        <v>199</v>
       </c>
       <c r="I3" s="2" t="str">
         <f>"Собеседования в 7-й математический класс 179-й школы"</f>
@@ -1668,14 +1660,14 @@
       </c>
       <c r="K3" t="str">
         <f t="shared" si="2"/>
-        <v>C:\Dropbox\M2021-sob\Собеседование в 7-й класс, 2017\_Задачи собеседований\sob10.pdf</v>
+        <v>C:\Dropbox\M2021-sob\Собеседование в 7-й класс, 2017\_Задачи собеседований\sob9.pdf</v>
       </c>
       <c r="M3" s="3" t="str">
         <f t="shared" si="3"/>
         <v>.</v>
       </c>
       <c r="N3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="O3">
         <v>0.82</v>
@@ -1702,89 +1694,89 @@
         <f t="shared" si="4"/>
         <v>10.130000000000001</v>
       </c>
-      <c r="X3" s="18" t="s">
+      <c r="X3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="Y3" s="18" t="s">
+      <c r="Y3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="Z3" s="18" t="s">
+      <c r="Z3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AA3" s="18" t="s">
+      <c r="AA3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AB3" s="18" t="s">
+      <c r="AB3" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="AC3" s="18" t="s">
+      <c r="AC3" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="AD3" s="18" t="s">
+      <c r="AD3" s="16" t="s">
         <v>188</v>
       </c>
       <c r="AF3" s="3">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="AG3" s="15" t="e">
+      <c r="AG3" s="13" t="e">
         <f>ROUND(IF(X3="+",1,IF(X3="+.",1,IF(X3="+-",0.8,IF(X3="+/2",0.5,IF(X3="-+",0.1,IF(X3="-.",0,IF(X3="-",0,IF(X3="0",0,IF(X3="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AH3" s="15" t="e">
+      <c r="AH3" s="13" t="e">
         <f>ROUND(IF(Y3="+",1,IF(Y3="+.",1,IF(Y3="+-",0.8,IF(Y3="+/2",0.5,IF(Y3="-+",0.1,IF(Y3="-.",0,IF(Y3="-",0,IF(Y3="0",0,IF(Y3="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AI3" s="15" t="e">
+      <c r="AI3" s="13" t="e">
         <f>ROUND(IF(Z3="+",1,IF(Z3="+.",1,IF(Z3="+-",0.8,IF(Z3="+/2",0.5,IF(Z3="-+",0.1,IF(Z3="-.",0,IF(Z3="-",0,IF(Z3="0",0,IF(Z3="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AJ3" s="15" t="e">
+      <c r="AJ3" s="13" t="e">
         <f>ROUND(IF(AA3="+",1,IF(AA3="+.",1,IF(AA3="+-",0.8,IF(AA3="+/2",0.5,IF(AA3="-+",0.1,IF(AA3="-.",0,IF(AA3="-",0,IF(AA3="0",0,IF(AA3="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AK3" s="15" t="e">
+      <c r="AK3" s="13" t="e">
         <f>ROUND(IF(AB3="+",1,IF(AB3="+.",1,IF(AB3="+-",0.8,IF(AB3="+/2",0.5,IF(AB3="-+",0.1,IF(AB3="-.",0,IF(AB3="-",0,IF(AB3="0",0,IF(AB3="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL3" s="15" t="e">
+      <c r="AL3" s="13" t="e">
         <f>ROUND(IF(AC3="+",1,IF(AC3="+.",1,IF(AC3="+-",0.8,IF(AC3="+/2",0.5,IF(AC3="-+",0.1,IF(AC3="-.",0,IF(AC3="-",0,IF(AC3="0",0,IF(AC3="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AM3" s="15" t="e">
+      <c r="AM3" s="13" t="e">
         <f>ROUND(IF(AD3="+",1,IF(AD3="+.",1,IF(AD3="+-",0.8,IF(AD3="+/2",0.5,IF(AD3="-+",0.1,IF(AD3="-.",0,IF(AD3="-",0,IF(AD3="0",0,IF(AD3="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AN3" s="15" t="e">
+      <c r="AN3" s="13" t="e">
         <f>ROUND(IF(AE3="+",1,IF(AE3="+.",1,IF(AE3="+-",0.8,IF(AE3="+/2",0.5,IF(AE3="-+",0.1,IF(AE3="-.",0,IF(AE3="-",0,IF(AE3="0",0,IF(AE3="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AO3" s="16" t="e">
+      <c r="AO3" s="14" t="e">
         <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>142</v>
       </c>
       <c r="B4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D4">
         <v>305</v>
       </c>
-      <c r="E4" t="s">
-        <v>199</v>
-      </c>
-      <c r="F4">
+      <c r="E4" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="F4" s="16">
         <v>2004</v>
       </c>
-      <c r="G4" s="20" t="s">
-        <v>208</v>
+      <c r="G4" s="18" t="s">
+        <v>205</v>
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" ref="I4:I5" si="7">"Собеседования в 7-й математический класс 179-й школы"</f>
@@ -1795,7 +1787,7 @@
         <v>|</v>
       </c>
       <c r="K4" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>"C:\Dropbox\M2021-sob\Собеседование в 7-й класс, 2017\_Задачи собеседований\sob10.pdf"</f>
         <v>C:\Dropbox\M2021-sob\Собеседование в 7-й класс, 2017\_Задачи собеседований\sob10.pdf</v>
       </c>
       <c r="L4" s="3"/>
@@ -1828,25 +1820,25 @@
         <f t="shared" si="4"/>
         <v>10.130000000000001</v>
       </c>
-      <c r="X4" s="18" t="s">
+      <c r="X4" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="Y4" s="18" t="s">
+      <c r="Y4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="Z4" s="18" t="s">
+      <c r="Z4" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="AA4" s="18" t="s">
+      <c r="AA4" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="AB4" s="18" t="s">
+      <c r="AB4" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="AC4" s="18" t="s">
+      <c r="AC4" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="AD4" s="18" t="s">
+      <c r="AD4" s="16" t="s">
         <v>188</v>
       </c>
       <c r="AF4" s="3">
@@ -1860,64 +1852,64 @@
 IF(AE4="+",1,IF(AE4="+.",1,IF(AE4="+-",0.8,IF(AE4="+/2",0.5,IF(AE4="-+",0.1,IF(AE4="-.",0,IF(AE4="-",0,IF(AE4="0",0,IF(AE4="",0,"?")))))))))</f>
         <v>1</v>
       </c>
-      <c r="AG4" s="14" t="e">
+      <c r="AG4" s="12" t="e">
         <f>ROUND(IF(X4="+",1,IF(X4="+.",1,IF(X4="+-",0.8,IF(X4="+/2",0.5,IF(X4="-+",0.1,IF(X4="-.",0,IF(X4="-",0,IF(X4="0",0,IF(X4="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AH4" s="15" t="e">
+      <c r="AH4" s="13" t="e">
         <f>ROUND(IF(Y4="+",1,IF(Y4="+.",1,IF(Y4="+-",0.8,IF(Y4="+/2",0.5,IF(Y4="-+",0.1,IF(Y4="-.",0,IF(Y4="-",0,IF(Y4="0",0,IF(Y4="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AI4" s="15" t="e">
+      <c r="AI4" s="13" t="e">
         <f>ROUND(IF(Z4="+",1,IF(Z4="+.",1,IF(Z4="+-",0.8,IF(Z4="+/2",0.5,IF(Z4="-+",0.1,IF(Z4="-.",0,IF(Z4="-",0,IF(Z4="0",0,IF(Z4="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AJ4" s="15" t="e">
+      <c r="AJ4" s="13" t="e">
         <f>ROUND(IF(AA4="+",1,IF(AA4="+.",1,IF(AA4="+-",0.8,IF(AA4="+/2",0.5,IF(AA4="-+",0.1,IF(AA4="-.",0,IF(AA4="-",0,IF(AA4="0",0,IF(AA4="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AK4" s="15" t="e">
+      <c r="AK4" s="13" t="e">
         <f>ROUND(IF(AB4="+",1,IF(AB4="+.",1,IF(AB4="+-",0.8,IF(AB4="+/2",0.5,IF(AB4="-+",0.1,IF(AB4="-.",0,IF(AB4="-",0,IF(AB4="0",0,IF(AB4="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL4" s="15" t="e">
+      <c r="AL4" s="13" t="e">
         <f>ROUND(IF(AC4="+",1,IF(AC4="+.",1,IF(AC4="+-",0.8,IF(AC4="+/2",0.5,IF(AC4="-+",0.1,IF(AC4="-.",0,IF(AC4="-",0,IF(AC4="0",0,IF(AC4="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AM4" s="15" t="e">
+      <c r="AM4" s="13" t="e">
         <f>ROUND(IF(AD4="+",1,IF(AD4="+.",1,IF(AD4="+-",0.8,IF(AD4="+/2",0.5,IF(AD4="-+",0.1,IF(AD4="-.",0,IF(AD4="-",0,IF(AD4="0",0,IF(AD4="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AN4" s="15" t="e">
+      <c r="AN4" s="13" t="e">
         <f>ROUND(IF(AE4="+",1,IF(AE4="+.",1,IF(AE4="+-",0.8,IF(AE4="+/2",0.5,IF(AE4="-+",0.1,IF(AE4="-.",0,IF(AE4="-",0,IF(AE4="0",0,IF(AE4="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AO4" s="17" t="e">
+      <c r="AO4" s="15" t="e">
         <f t="shared" ref="AO4:AO5" si="11">ROUND(SUM(AG4:AN4),2)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" t="s">
         <v>192</v>
-      </c>
-      <c r="B5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C5" t="s">
-        <v>193</v>
       </c>
       <c r="D5">
         <v>305</v>
       </c>
-      <c r="E5" t="s">
-        <v>194</v>
-      </c>
-      <c r="F5">
+      <c r="E5" s="16">
+        <v>368</v>
+      </c>
+      <c r="F5" s="16">
         <v>2004</v>
       </c>
-      <c r="G5" s="20" t="s">
-        <v>203</v>
+      <c r="G5" s="18" t="s">
+        <v>200</v>
       </c>
       <c r="H5" t="s">
         <v>87</v>
@@ -1932,7 +1924,7 @@
       </c>
       <c r="K5" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>C:\Dropbox\M2021-sob\Собеседование в 7-й класс, 2017\_Задачи собеседований\sob10.pdf</v>
+        <v>C:\Dropbox\M2021-sob\Собеседование в 7-й класс, 2017\_Задачи собеседований\sob9.pdf</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3" t="str">
@@ -1964,70 +1956,70 @@
         <f t="shared" si="4"/>
         <v>10.130000000000001</v>
       </c>
-      <c r="X5" s="18" t="s">
+      <c r="X5" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="Y5" s="18" t="s">
+      <c r="Y5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="Z5" s="18" t="s">
+      <c r="Z5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AA5" s="18" t="s">
+      <c r="AA5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AB5" s="18" t="s">
+      <c r="AB5" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="AC5" s="18" t="s">
+      <c r="AC5" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="AD5" s="18" t="s">
+      <c r="AD5" s="16" t="s">
         <v>20</v>
       </c>
       <c r="AF5" s="3">
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
-      <c r="AG5" s="14" t="e">
+      <c r="AG5" s="12" t="e">
         <f>ROUND(IF(X5="+",1,IF(X5="+.",1,IF(X5="+-",0.8,IF(X5="+/2",0.5,IF(X5="-+",0.1,IF(X5="-.",0,IF(X5="-",0,IF(X5="0",0,IF(X5="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AH5" s="15" t="e">
+      <c r="AH5" s="13" t="e">
         <f>ROUND(IF(Y5="+",1,IF(Y5="+.",1,IF(Y5="+-",0.8,IF(Y5="+/2",0.5,IF(Y5="-+",0.1,IF(Y5="-.",0,IF(Y5="-",0,IF(Y5="0",0,IF(Y5="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AI5" s="15" t="e">
+      <c r="AI5" s="13" t="e">
         <f>ROUND(IF(Z5="+",1,IF(Z5="+.",1,IF(Z5="+-",0.8,IF(Z5="+/2",0.5,IF(Z5="-+",0.1,IF(Z5="-.",0,IF(Z5="-",0,IF(Z5="0",0,IF(Z5="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AJ5" s="15" t="e">
+      <c r="AJ5" s="13" t="e">
         <f>ROUND(IF(AA5="+",1,IF(AA5="+.",1,IF(AA5="+-",0.8,IF(AA5="+/2",0.5,IF(AA5="-+",0.1,IF(AA5="-.",0,IF(AA5="-",0,IF(AA5="0",0,IF(AA5="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AK5" s="15" t="e">
+      <c r="AK5" s="13" t="e">
         <f>ROUND(IF(AB5="+",1,IF(AB5="+.",1,IF(AB5="+-",0.8,IF(AB5="+/2",0.5,IF(AB5="-+",0.1,IF(AB5="-.",0,IF(AB5="-",0,IF(AB5="0",0,IF(AB5="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL5" s="15" t="e">
+      <c r="AL5" s="13" t="e">
         <f>ROUND(IF(AC5="+",1,IF(AC5="+.",1,IF(AC5="+-",0.8,IF(AC5="+/2",0.5,IF(AC5="-+",0.1,IF(AC5="-.",0,IF(AC5="-",0,IF(AC5="0",0,IF(AC5="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AM5" s="15" t="e">
+      <c r="AM5" s="13" t="e">
         <f>ROUND(IF(AD5="+",1,IF(AD5="+.",1,IF(AD5="+-",0.8,IF(AD5="+/2",0.5,IF(AD5="-+",0.1,IF(AD5="-.",0,IF(AD5="-",0,IF(AD5="0",0,IF(AD5="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AN5" s="15" t="e">
+      <c r="AN5" s="13" t="e">
         <f>ROUND(IF(AE5="+",1,IF(AE5="+.",1,IF(AE5="+-",0.8,IF(AE5="+/2",0.5,IF(AE5="-+",0.1,IF(AE5="-.",0,IF(AE5="-",0,IF(AE5="0",0,IF(AE5="",0,"?")))))))))*#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="AO5" s="17" t="e">
+      <c r="AO5" s="15" t="e">
         <f t="shared" si="11"/>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="E8" s="19"/>
+    <row r="8" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E8" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2037,7 +2029,7 @@
     <hyperlink ref="G5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <legacyDrawing r:id="rId6"/>
   <tableParts count="1">
     <tablePart r:id="rId7"/>
@@ -2053,12 +2045,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -2066,7 +2058,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -2074,7 +2066,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -2082,7 +2074,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2090,7 +2082,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -2098,7 +2090,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -2106,7 +2098,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -2114,7 +2106,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -2122,7 +2114,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>76</v>
       </c>
@@ -2130,7 +2122,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -2138,7 +2130,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -2146,7 +2138,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -2154,7 +2146,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -2162,7 +2154,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -2170,7 +2162,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -2178,7 +2170,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -2186,7 +2178,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>107</v>
       </c>
@@ -2194,7 +2186,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>109</v>
       </c>
@@ -2202,7 +2194,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>111</v>
       </c>
@@ -2210,7 +2202,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -2218,7 +2210,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -2226,7 +2218,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -2234,7 +2226,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>116</v>
       </c>
@@ -2242,7 +2234,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -2250,7 +2242,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -2258,7 +2250,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>120</v>
       </c>
@@ -2266,7 +2258,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>122</v>
       </c>
@@ -2274,7 +2266,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>124</v>
       </c>
@@ -2282,7 +2274,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -2290,7 +2282,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>127</v>
       </c>
@@ -2298,7 +2290,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>129</v>
       </c>
@@ -2306,7 +2298,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -2314,7 +2306,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -2322,7 +2314,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2330,7 +2322,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -2338,7 +2330,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -2346,7 +2338,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -2354,7 +2346,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>137</v>
       </c>
@@ -2362,7 +2354,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -2370,7 +2362,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>140</v>
       </c>
@@ -2378,7 +2370,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>142</v>
       </c>
@@ -2386,7 +2378,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>72</v>
       </c>
@@ -2394,7 +2386,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -2402,7 +2394,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>146</v>
       </c>
@@ -2410,7 +2402,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>148</v>
       </c>
@@ -2418,7 +2410,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -2426,7 +2418,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -2434,7 +2426,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>152</v>
       </c>
@@ -2442,7 +2434,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>59</v>
       </c>
@@ -2450,7 +2442,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>23</v>
       </c>
@@ -2458,7 +2450,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -2466,7 +2458,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -2474,7 +2466,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>43</v>
       </c>
@@ -2482,7 +2474,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2490,7 +2482,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -2498,7 +2490,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>161</v>
       </c>
@@ -2506,7 +2498,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>44</v>
       </c>
@@ -2514,7 +2506,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>164</v>
       </c>
@@ -2522,7 +2514,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -2530,7 +2522,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>27</v>
       </c>
@@ -2538,7 +2530,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -2546,7 +2538,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>169</v>
       </c>
@@ -2554,7 +2546,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>56</v>
       </c>
@@ -2562,7 +2554,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>29</v>
       </c>
@@ -2570,7 +2562,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -2578,7 +2570,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>174</v>
       </c>
@@ -2586,7 +2578,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -2594,7 +2586,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>64</v>
       </c>
@@ -2602,7 +2594,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>55</v>
       </c>
@@ -2610,7 +2602,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>179</v>
       </c>
@@ -2618,7 +2610,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>181</v>
       </c>
@@ -2626,7 +2618,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>183</v>
       </c>
@@ -2634,7 +2626,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>185</v>
       </c>

</xml_diff>